<commit_message>
add database handler test
</commit_message>
<xml_diff>
--- a/Tools/FrameworkTestPlan.xlsx
+++ b/Tools/FrameworkTestPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\github\BIADemo\Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\Github.com\BIATeam\BIADemo\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46E0A81-FAA0-4F40-9908-FF3FC22722CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ABD662-96E9-45CD-A532-90F66A2EAB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{504142AA-995E-448E-B899-958ED8504F94}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{504142AA-995E-448E-B899-958ED8504F94}"/>
   </bookViews>
   <sheets>
     <sheet name="FMK fct val" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="144">
   <si>
     <t>Framework functional validation</t>
   </si>
@@ -467,6 +467,21 @@
   </si>
   <si>
     <t>Readonly data (in row and in popup form)</t>
+  </si>
+  <si>
+    <t>Database Handler</t>
+  </si>
+  <si>
+    <t>Worker service database handker</t>
+  </si>
+  <si>
+    <t>Open the plane list and active option "Always up to date"
+Touche a plane in SSMS:
+UPDATE [dbo].[Planes]
+   SET [Msn] = 'MSN300038T'
+ WHERE Id=38
+GO
+Verify that the screen is automaticaly refreshed with the new value.</t>
   </si>
 </sst>
 </file>
@@ -1139,15 +1154,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71440E81-3ABF-488E-A0D4-CD21439D0B0F}">
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A95" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" style="7" customWidth="1"/>
     <col min="4" max="4" width="38.7109375" customWidth="1"/>
     <col min="5" max="5" width="69.85546875" customWidth="1"/>
@@ -2196,168 +2212,186 @@
       <c r="E128" s="15"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="23"/>
-      <c r="B129" s="23"/>
-      <c r="C129" s="22">
+      <c r="A129" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B129" s="29"/>
+      <c r="C129" s="20"/>
+      <c r="D129" s="21"/>
+    </row>
+    <row r="130" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B130" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C130" s="18"/>
+      <c r="D130" s="19"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="23"/>
+      <c r="B131" s="23"/>
+      <c r="C131" s="22">
         <f>COUNTIF(C9:C128,"&gt;&lt;NOT APPLICABLE")</f>
         <v>0</v>
       </c>
-      <c r="D129" s="24">
-        <f>SUM(D130:D134)</f>
+      <c r="D131" s="24">
+        <f>SUM(D132:D136)</f>
         <v>0</v>
       </c>
-      <c r="E129" s="16"/>
-    </row>
-    <row r="130" spans="1:5" ht="34.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130" s="18" t="s">
+      <c r="E131" s="16"/>
+    </row>
+    <row r="132" spans="1:5" ht="34.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B130" s="22"/>
-      <c r="C130" s="27" t="e">
-        <f>(COUNTIF(C8:C128,"PASSED"))/C129</f>
+      <c r="B132" s="22"/>
+      <c r="C132" s="27" t="e">
+        <f>(COUNTIF(C8:C128,"PASSED"))/C131</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D130" s="26">
+      <c r="D132" s="26">
         <f>COUNTIF(C8:C128,"PASSED")</f>
         <v>0</v>
       </c>
-      <c r="E130" s="16"/>
-    </row>
-    <row r="131" spans="1:5" ht="34.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" s="18" t="s">
+      <c r="E132" s="16"/>
+    </row>
+    <row r="133" spans="1:5" ht="34.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B131" s="22"/>
-      <c r="C131" s="28" t="e">
-        <f>(COUNTIF(C9:C128,"FAILED"))/C129</f>
+      <c r="B133" s="22"/>
+      <c r="C133" s="28" t="e">
+        <f>(COUNTIF(C9:C128,"FAILED"))/C131</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D131" s="26">
+      <c r="D133" s="26">
         <f>COUNTIF(C9:C128,"FAILED")</f>
         <v>0</v>
       </c>
-      <c r="E131" s="16"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="18" t="s">
+      <c r="E133" s="16"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B132" s="22"/>
-      <c r="C132" s="25" t="e">
-        <f>(COUNTIF(C10:C128,"NOT TESTED"))/C129</f>
+      <c r="B134" s="22"/>
+      <c r="C134" s="25" t="e">
+        <f>(COUNTIF(C10:C128,"NOT TESTED"))/C131</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D132" s="26">
+      <c r="D134" s="26">
         <f>COUNTIF(C10:C128,"NOT TESTED")</f>
         <v>0</v>
       </c>
-      <c r="E132" s="16"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B133" s="22"/>
-      <c r="C133" s="25" t="e">
-        <f>(COUNTIF(C11:C131,"BLOCKED"))/C129</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D133" s="26">
-        <f>COUNTIF(C11:C131,"BLOCKED")</f>
-        <v>0</v>
-      </c>
-      <c r="E133" s="16"/>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="B134" s="22"/>
-      <c r="C134" s="25" t="e">
-        <f>(COUNTIF(C12:C132,"IN PROGRESS"))/C129</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D134" s="26">
-        <f>COUNTIF(C12:C132,"IN PROGRESS")</f>
-        <v>0</v>
-      </c>
       <c r="E134" s="16"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="18" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="B135" s="22"/>
       <c r="C135" s="25" t="e">
-        <f>(COUNTIF(C12:C133,"ON HOLD"))/C129</f>
+        <f>(COUNTIF(C11:C133,"BLOCKED"))/C131</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D135" s="26">
-        <f>COUNTIF(C12:C133,"ON HOLD")</f>
+        <f>COUNTIF(C11:C133,"BLOCKED")</f>
         <v>0</v>
       </c>
       <c r="E135" s="16"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="18" t="s">
-        <v>18</v>
+        <v>129</v>
       </c>
       <c r="B136" s="22"/>
       <c r="C136" s="25" t="e">
-        <f>(COUNTIF(C13:C134,"NOT APPLICABLE"))/(COUNTA(C9:C128))</f>
+        <f>(COUNTIF(C12:C134,"IN PROGRESS"))/C131</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D136" s="26">
-        <f>COUNTIF(C13:C134,"NOT APPLICABLE")</f>
+        <f>COUNTIF(C12:C134,"IN PROGRESS")</f>
         <v>0</v>
       </c>
       <c r="E136" s="16"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C137" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D137" t="s">
-        <v>130</v>
+      <c r="A137" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B137" s="22"/>
+      <c r="C137" s="25" t="e">
+        <f>(COUNTIF(C12:C135,"ON HOLD"))/C131</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D137" s="26">
+        <f>COUNTIF(C12:C135,"ON HOLD")</f>
+        <v>0</v>
       </c>
       <c r="E137" s="16"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C138" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D138" t="s">
-        <v>5</v>
-      </c>
+      <c r="A138" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B138" s="22"/>
+      <c r="C138" s="25" t="e">
+        <f>(COUNTIF(C13:C136,"NOT APPLICABLE"))/(COUNTA(C9:C128))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D138" s="26">
+        <f>COUNTIF(C13:C136,"NOT APPLICABLE")</f>
+        <v>0</v>
+      </c>
+      <c r="E138" s="16"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C139" s="7" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="D139" t="s">
-        <v>131</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="E139" s="16"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C140" s="7" t="s">
-        <v>129</v>
+        <v>7</v>
       </c>
       <c r="D140" t="s">
-        <v>132</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C141" s="7" t="s">
-        <v>89</v>
+        <v>33</v>
+      </c>
+      <c r="D141" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C142" s="7" t="s">
-        <v>18</v>
+        <v>129</v>
+      </c>
+      <c r="D142" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C143" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C144" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="7" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2366,9 +2400,9 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="A130:B136">
+  <conditionalFormatting sqref="A132:B138">
     <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="FAILED">
-      <formula>NOT(ISERROR(SEARCH("FAILED",A130)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FAILED",A132)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"PASSED"</formula>
@@ -2412,7 +2446,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C129">
+  <conditionalFormatting sqref="C8:C131">
     <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="FAILED">
       <formula>NOT(ISERROR(SEARCH("FAILED",C8)))</formula>
     </cfRule>
@@ -2420,7 +2454,7 @@
       <formula>"PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:C129">
+  <conditionalFormatting sqref="C9:C131">
     <cfRule type="colorScale" priority="179">
       <colorScale>
         <cfvo type="min"/>
@@ -2442,10 +2476,10 @@
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5" xr:uid="{907BF470-8617-4B57-828B-5E621626793C}">
-      <formula1>$D$137:$D$139</formula1>
+      <formula1>$D$139:$D$141</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C128" xr:uid="{901B4090-8C53-44BA-A7CE-3694A5F24D66}">
-      <formula1>$C$137:$C$143</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C130" xr:uid="{901B4090-8C53-44BA-A7CE-3694A5F24D66}">
+      <formula1>$C$139:$C$145</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2458,8 +2492,8 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="3" operator="containsText" id="{CF073450-DF97-4CEA-B330-C954CD06556B}">
-            <xm:f>NOT(ISERROR(SEARCH($C$140,A130)))</xm:f>
-            <xm:f>$C$140</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$142,A132)))</xm:f>
+            <xm:f>$C$142</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2469,8 +2503,8 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="4" operator="containsText" id="{3F8DC7E6-6705-411A-8075-C53360946CC7}">
-            <xm:f>NOT(ISERROR(SEARCH($C$137,A130)))</xm:f>
-            <xm:f>$C$137</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$139,A132)))</xm:f>
+            <xm:f>$C$139</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2480,8 +2514,8 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="7" operator="containsText" id="{7DE7F85E-C17A-4D12-8F3C-038A7427C9F9}">
-            <xm:f>NOT(ISERROR(SEARCH($C$143,A130)))</xm:f>
-            <xm:f>$C$143</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$145,A132)))</xm:f>
+            <xm:f>$C$145</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FFFF0000"/>
@@ -2493,12 +2527,12 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A130:B136</xm:sqref>
+          <xm:sqref>A132:B138</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="80" operator="containsText" id="{89D2785E-E162-4001-865C-F6BBBA578578}">
-            <xm:f>NOT(ISERROR(SEARCH($C$143,C1)))</xm:f>
-            <xm:f>$C$143</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$145,C1)))</xm:f>
+            <xm:f>$C$145</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FFFF0000"/>
@@ -2510,12 +2544,12 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C137:C1048576 C1:C129</xm:sqref>
+          <xm:sqref>C139:C1048576 C1:C131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="177" operator="containsText" id="{D9C9BAE0-E428-42EB-ACD3-CDB9F6864B86}">
-            <xm:f>NOT(ISERROR(SEARCH($C$140,C9)))</xm:f>
-            <xm:f>$C$140</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$142,C9)))</xm:f>
+            <xm:f>$C$142</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2525,8 +2559,8 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="containsText" priority="178" operator="containsText" id="{D19F0B1D-AB64-4BBA-B677-5A1B402A0E0C}">
-            <xm:f>NOT(ISERROR(SEARCH($C$137,C9)))</xm:f>
-            <xm:f>$C$137</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH($C$139,C9)))</xm:f>
+            <xm:f>$C$139</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2535,7 +2569,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C9:C129</xm:sqref>
+          <xm:sqref>C9:C131</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2792,6 +2826,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="64899395-4b02-4b78-9a08-b88d79b1e06c">
@@ -2801,15 +2844,6 @@
     <TaxCatchAll xmlns="1af08207-2f6c-4c0b-b1de-643deecae290" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2832,6 +2866,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B3D449-99D9-4EDB-A3A6-1774D2F10211}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A680A5-FECB-4E1C-999F-11358A60826B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -2846,12 +2888,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8B3D449-99D9-4EDB-A3A6-1774D2F10211}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>